<commit_message>
apply all latest sample project changes since 11/06
</commit_message>
<xml_diff>
--- a/src/main/resources/com/company/library/reports/new/Template for publications by type.xlsx
+++ b/src/main/resources/com/company/library/reports/new/Template for publications by type.xlsx
@@ -333,13 +333,13 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.73"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>

</xml_diff>